<commit_message>
https://jira.aplana.com/browse/SBRFNDFL-4767 Патч БД 3.0
</commit_message>
<xml_diff>
--- a/database/database-3.0/templates/data/ndfl/primary_rnu_ndfl/v2016/excel_template_dec.xlsx
+++ b/database/database-3.0/templates/data/ndfl/primary_rnu_ndfl/v2016/excel_template_dec.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Apronin\IdeaProject\sbrfndfl\db\changelog\templates\ndfl\primary_rnu_ndfl\v2016\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Правила заполнения" sheetId="2" r:id="rId1"/>
     <sheet name="РНУ НДФЛ" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -222,36 +227,36 @@
     <t>Особенности заполнения</t>
   </si>
   <si>
+    <t>Столбец №23 "ID операции"</t>
+  </si>
+  <si>
+    <t>СведАванс. ID операции</t>
+  </si>
+  <si>
+    <t>НДФЛ возвращённый НП</t>
+  </si>
+  <si>
+    <t>Дата платёжного поручения</t>
+  </si>
+  <si>
+    <t>Номер платёжного поручения</t>
+  </si>
+  <si>
+    <t>Сумма платёжного поручения</t>
+  </si>
+  <si>
     <t>1. При отсутствии информации об ID операции необходимо указывать обозначение операции, уникальное в рамках данного файла.
-Уникальное обозначение необходимо указывать для групп строк по начислению, корректировке начисления, выплате и перечислению в бюджет относящиеся к одной операции.
+Уникальное обозначение необходимо указывать для групп строк по начислению, выплате и перечислению в бюджет относящиеся к одной операции.
 При загрузке файла Система будет находить строки с одинаковыми значениями в столбце «ID операции» и преобразовывать их в номер по определённому алгоритму.
 2. При внесении изменений в операции предыдущего периода необходимо выгрузить данные с предыдущей формы и дополнить его новыми данными.
 В новых строках указывать ID операции, присвоенных при загрузке предыдущих данных.</t>
-  </si>
-  <si>
-    <t>Столбец №23 "ID операции"</t>
-  </si>
-  <si>
-    <t>СведАванс. ID операции</t>
-  </si>
-  <si>
-    <t>НДФЛ возвращённый НП</t>
-  </si>
-  <si>
-    <t>Дата платёжного поручения</t>
-  </si>
-  <si>
-    <t>Номер платёжного поручения</t>
-  </si>
-  <si>
-    <t>Сумма платёжного поручения</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,30 +684,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.5703125" customWidth="1"/>
     <col min="2" max="2" width="88" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="21">
+    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>60</v>
       </c>
@@ -710,12 +717,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="210">
+    <row r="5" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -725,17 +732,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="52.5">
+    <row r="1" spans="1:64" ht="52.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>58</v>
       </c>
@@ -857,19 +864,19 @@
         <v>38</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="AQ1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="AT1" s="4" t="s">
         <v>40</v>
@@ -914,7 +921,7 @@
         <v>51</v>
       </c>
       <c r="BH1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BI1" s="4" t="s">
         <v>52</v>
@@ -929,7 +936,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:64">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>0</v>
       </c>

</xml_diff>